<commit_message>
Made changes to the logic for the queue manager and the poltting
</commit_message>
<xml_diff>
--- a/Pulse_Manager.xlsx
+++ b/Pulse_Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MPQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4BA8AD-61A8-4B4D-A549-2A011316A005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A447ED-D8CF-449D-B2B4-5735EC37F537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pulse_Queue" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="40">
   <si>
     <t>Pulse_1</t>
   </si>
@@ -124,9 +124,6 @@
     <t>Start Time</t>
   </si>
   <si>
-    <t>End Time</t>
-  </si>
-  <si>
     <t>On</t>
   </si>
   <si>
@@ -143,6 +140,12 @@
   </si>
   <si>
     <t>Pulse_4</t>
+  </si>
+  <si>
+    <t>Pulse Length</t>
+  </si>
+  <si>
+    <t>Pulse_5</t>
   </si>
 </sst>
 </file>
@@ -466,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FB8CB8-4733-4C3F-877C-69E1CF4DE4A4}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -487,7 +490,7 @@
         <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -503,7 +506,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3">
         <v>80</v>
@@ -514,7 +517,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4">
         <v>20</v>
@@ -525,7 +528,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5">
         <v>110</v>
@@ -536,13 +539,24 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>400</v>
       </c>
       <c r="C6">
         <v>440</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7">
+        <v>320</v>
+      </c>
+      <c r="C7">
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -552,71 +566,80 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.453125" customWidth="1"/>
     <col min="2" max="2" width="10.26953125" customWidth="1"/>
-    <col min="3" max="5" width="10.08984375" customWidth="1"/>
+    <col min="3" max="6" width="10.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
         <v>37</v>
       </c>
-      <c r="E1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -624,7 +647,7 @@
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
         <v>30</v>
@@ -632,8 +655,11 @@
       <c r="E4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -647,15 +673,18 @@
         <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
         <v>30</v>
@@ -666,8 +695,11 @@
       <c r="E6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -683,8 +715,11 @@
       <c r="E7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -700,8 +735,11 @@
       <c r="E8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -717,8 +755,11 @@
       <c r="E9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -734,8 +775,11 @@
       <c r="E10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -751,8 +795,11 @@
       <c r="E11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -768,8 +815,11 @@
       <c r="E12" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -785,8 +835,11 @@
       <c r="E13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -802,8 +855,11 @@
       <c r="E14" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -819,8 +875,11 @@
       <c r="E15" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -836,8 +895,11 @@
       <c r="E16" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -853,8 +915,11 @@
       <c r="E17" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -870,8 +935,11 @@
       <c r="E18" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -887,8 +955,11 @@
       <c r="E19" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -904,8 +975,11 @@
       <c r="E20" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -921,8 +995,11 @@
       <c r="E21" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -938,8 +1015,11 @@
       <c r="E22" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -955,8 +1035,11 @@
       <c r="E23" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -972,8 +1055,11 @@
       <c r="E24" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -989,8 +1075,11 @@
       <c r="E25" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1006,8 +1095,11 @@
       <c r="E26" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1023,8 +1115,11 @@
       <c r="E27" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1040,8 +1135,11 @@
       <c r="E28" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1055,13 +1153,16 @@
         <v>30</v>
       </c>
       <c r="E29" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:E29" xr:uid="{691C8B71-F12B-4438-A5DE-05B4BE4A1351}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:F29" xr:uid="{691C8B71-F12B-4438-A5DE-05B4BE4A1351}">
       <formula1>"On, Sweep, Off"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>